<commit_message>
chore: update glossary exports
</commit_message>
<xml_diff>
--- a/exports/xlsx/terms_definition_1.xlsx
+++ b/exports/xlsx/terms_definition_1.xlsx
@@ -1809,8 +1809,8 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>- The subset may be spatial, temporal, spectral, or in any other dimension or Trait.
-- The subset is contiguous, i.e. it does not consist of more than one discontinuous interval along any dimension.
+          <t>- A sample may be spatial, temporal, spectral, or in any other dimension or Trait.
+- Each sample is contiguous, i.e. it does not consist of more than one discontinuous geometry in any dimension.
 - The Process of obtaining a sample is called sampling.</t>
         </is>
       </c>

</xml_diff>